<commit_message>
Some import vendor billing tracker changes
</commit_message>
<xml_diff>
--- a/modules/purchase/uploads/file_sample/Sample_vendor_billing_tracker_item_en.xlsx
+++ b/modules/purchase/uploads/file_sample/Sample_vendor_billing_tracker_item_en.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t xml:space="preserve"> Invoice number</t>
   </si>
@@ -39,16 +39,13 @@
     <t>(*)Description of Services</t>
   </si>
   <si>
-    <t>Amount w/o Tax</t>
-  </si>
-  <si>
-    <t>Tax Value</t>
-  </si>
-  <si>
-    <t>Total included tax</t>
-  </si>
-  <si>
-    <t>Certified Amount</t>
+    <t xml:space="preserve"> Invoice Code</t>
+  </si>
+  <si>
+    <t>Certified Amount w/o Tax</t>
+  </si>
+  <si>
+    <t>Certified Tax Amount</t>
   </si>
 </sst>
 </file>
@@ -393,7 +390,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -401,10 +398,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J1"/>
+  <dimension ref="A1:I1"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="15"/>
@@ -418,40 +415,36 @@
     <col min="7" max="7" width="40.28515625" style="3" customWidth="1"/>
     <col min="8" max="8" width="24" style="3" customWidth="1"/>
     <col min="9" max="9" width="25.140625" style="3" customWidth="1"/>
-    <col min="10" max="10" width="17.28515625" style="3" customWidth="1"/>
-    <col min="11" max="16384" width="9.28515625" style="3"/>
+    <col min="10" max="16384" width="9.28515625" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="2" customFormat="1" ht="50.25" customHeight="1">
+    <row r="1" spans="1:9" s="2" customFormat="1" ht="50.25" customHeight="1">
       <c r="A1" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="C1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="D1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="E1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="F1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="G1" s="4" t="s">
         <v>5</v>
-      </c>
-      <c r="G1" s="4" t="s">
-        <v>6</v>
       </c>
       <c r="H1" s="4" t="s">
         <v>7</v>
       </c>
       <c r="I1" s="4" t="s">
         <v>8</v>
-      </c>
-      <c r="J1" s="4" t="s">
-        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>